<commit_message>
added positive findings to videos in he and helist in he
</commit_message>
<xml_diff>
--- a/g6-06-he/helist.xlsx
+++ b/g6-06-he/helist.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Technische Universität Graz\Studium\4. Semester\HCI\hci_06_06\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\OneDrive - Technische Universität Graz\Studium\4. Semester\HCI\hci_06_06\g6-06-he\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A7D85BC-EFBB-4081-A496-E46D3BB1DBED}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98AD978A-B86E-4EEE-B1D3-338AE21BF191}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="4215" windowWidth="21600" windowHeight="11385" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-10755" yWindow="2070" windowWidth="21600" windowHeight="11385" tabRatio="500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Problems" sheetId="1" r:id="rId1"/>
@@ -184,7 +184,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="640" uniqueCount="443">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="634" uniqueCount="453">
   <si>
     <t>Heuristic Evaluation Results</t>
   </si>
@@ -1311,24 +1311,12 @@
     <t>Contacts -&gt; Email</t>
   </si>
   <si>
-    <t>lk-pc-pos03-Webcam.mp4</t>
-  </si>
-  <si>
     <t>There's a nice interactive webcam on the side. It shoes you a live feed of the best view of Graz.</t>
   </si>
   <si>
     <t>ml-pc-pos02-webcam-feature.mp4,  ms-pc-pos02-live-webcams.mp4, lk-pc-pos03-Webcam.mp4</t>
   </si>
   <si>
-    <t>ml-mob-pos01-top-event-slide.mp5</t>
-  </si>
-  <si>
-    <t>ms-pc-pos03-keywords-are-links.mp4</t>
-  </si>
-  <si>
-    <t>ms-pc-pos01-information.mp4</t>
-  </si>
-  <si>
     <t>n10-ml-pc-neg11-dead-link.mp4</t>
   </si>
   <si>
@@ -1546,6 +1534,48 @@
   </si>
   <si>
     <t xml:space="preserve"> ms-pc-neg05-interactive-map-filter.mp4, lk-pc-neg06-MapErrorUncheckl.mp4</t>
+  </si>
+  <si>
+    <t>p01-ml-mob-pos01-top-event-slide.mp4</t>
+  </si>
+  <si>
+    <t>p02-ml-pc-pos03-interactive-city-plan.mp4</t>
+  </si>
+  <si>
+    <t>p03-ms-pc-pos03-keywords-are-links.mp4</t>
+  </si>
+  <si>
+    <t>p04-mm-pc-pos03-groups.mp4</t>
+  </si>
+  <si>
+    <t>p05-ml-mob-pos03-top-ten-attractions.mp4</t>
+  </si>
+  <si>
+    <t>p06-ms-pc-pos01-information.mp4</t>
+  </si>
+  <si>
+    <t>p07-mm-pc-pos01-search.mp4</t>
+  </si>
+  <si>
+    <t>p08-lk-pc-pos03-Webcam.mp4</t>
+  </si>
+  <si>
+    <t>p09-ms-mob-pos01-easy-navigation.mp4</t>
+  </si>
+  <si>
+    <t>p10-mm-pc-pos02-advent.mp4</t>
+  </si>
+  <si>
+    <t>p11-lk-pc-pos01-Email.mp4</t>
+  </si>
+  <si>
+    <t>p12-ms-mob-pos02-bookmarks-working.mp4</t>
+  </si>
+  <si>
+    <t>p13-lk-mob-pos01-Webcam.mp4</t>
+  </si>
+  <si>
+    <t>p14-lk-pc-pos02-CloseMap.mp4</t>
   </si>
 </sst>
 </file>
@@ -1685,7 +1715,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
@@ -1810,6 +1840,7 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2126,7 +2157,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AG82"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A16" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
@@ -2235,7 +2266,7 @@
         <v>350</v>
       </c>
       <c r="D5" s="17" t="s">
-        <v>429</v>
+        <v>425</v>
       </c>
       <c r="E5" s="17" t="s">
         <v>351</v>
@@ -2264,7 +2295,7 @@
         <v>4</v>
       </c>
       <c r="Q5" s="23">
-        <f>SUM(M5:P5)/4</f>
+        <f t="shared" ref="Q5:Q36" si="0">SUM(M5:P5)/4</f>
         <v>3.75</v>
       </c>
     </row>
@@ -2279,7 +2310,7 @@
         <v>127</v>
       </c>
       <c r="D6" s="36" t="s">
-        <v>430</v>
+        <v>426</v>
       </c>
       <c r="E6" s="18" t="s">
         <v>128</v>
@@ -2310,7 +2341,7 @@
         <v>4</v>
       </c>
       <c r="Q6" s="23">
-        <f>SUM(M6:P6)/4</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -2325,7 +2356,7 @@
         <v>148</v>
       </c>
       <c r="D7" s="17" t="s">
-        <v>435</v>
+        <v>431</v>
       </c>
       <c r="E7" s="17" t="s">
         <v>149</v>
@@ -2356,7 +2387,7 @@
         <v>3</v>
       </c>
       <c r="Q7" s="23">
-        <f>SUM(M7:P7)/4</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -2371,7 +2402,7 @@
         <v>210</v>
       </c>
       <c r="D8" s="17" t="s">
-        <v>431</v>
+        <v>427</v>
       </c>
       <c r="E8" s="17" t="s">
         <v>211</v>
@@ -2402,7 +2433,7 @@
         <v>3</v>
       </c>
       <c r="Q8" s="23">
-        <f>SUM(M8:P8)/4</f>
+        <f t="shared" si="0"/>
         <v>3.5</v>
       </c>
     </row>
@@ -2417,7 +2448,7 @@
         <v>56</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>436</v>
+        <v>432</v>
       </c>
       <c r="E9" s="18" t="s">
         <v>57</v>
@@ -2448,7 +2479,7 @@
         <v>3</v>
       </c>
       <c r="Q9" s="23">
-        <f>SUM(M9:P9)/4</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
@@ -2463,7 +2494,7 @@
         <v>89</v>
       </c>
       <c r="D10" s="17" t="s">
-        <v>432</v>
+        <v>428</v>
       </c>
       <c r="E10" s="17" t="s">
         <v>90</v>
@@ -2494,7 +2525,7 @@
         <v>4</v>
       </c>
       <c r="Q10" s="23">
-        <f>SUM(M10:P10)/4</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
@@ -2509,7 +2540,7 @@
         <v>124</v>
       </c>
       <c r="D11" s="17" t="s">
-        <v>437</v>
+        <v>433</v>
       </c>
       <c r="E11" s="17" t="s">
         <v>315</v>
@@ -2542,7 +2573,7 @@
         <v>3</v>
       </c>
       <c r="Q11" s="23">
-        <f>SUM(M11:P11)/4</f>
+        <f t="shared" si="0"/>
         <v>3.25</v>
       </c>
     </row>
@@ -2557,7 +2588,7 @@
         <v>60</v>
       </c>
       <c r="D12" s="18" t="s">
-        <v>433</v>
+        <v>429</v>
       </c>
       <c r="E12" s="18" t="s">
         <v>61</v>
@@ -2586,7 +2617,7 @@
         <v>3</v>
       </c>
       <c r="Q12" s="23">
-        <f>SUM(M12:P12)/4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -2601,7 +2632,7 @@
         <v>139</v>
       </c>
       <c r="D13" s="17" t="s">
-        <v>434</v>
+        <v>430</v>
       </c>
       <c r="E13" s="17" t="s">
         <v>140</v>
@@ -2632,7 +2663,7 @@
         <v>2</v>
       </c>
       <c r="Q13" s="23">
-        <f>SUM(M13:P13)/4</f>
+        <f t="shared" si="0"/>
         <v>3</v>
       </c>
     </row>
@@ -2647,7 +2678,7 @@
         <v>64</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>370</v>
+        <v>366</v>
       </c>
       <c r="E14" s="18" t="s">
         <v>65</v>
@@ -2678,7 +2709,7 @@
         <v>2</v>
       </c>
       <c r="Q14" s="23">
-        <f>SUM(M14:P14)/4</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -2693,7 +2724,7 @@
         <v>96</v>
       </c>
       <c r="D15" s="17" t="s">
-        <v>371</v>
+        <v>367</v>
       </c>
       <c r="E15" s="17" t="s">
         <v>97</v>
@@ -2724,7 +2755,7 @@
         <v>2</v>
       </c>
       <c r="Q15" s="23">
-        <f>SUM(M15:P15)/4</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -2739,7 +2770,7 @@
         <v>135</v>
       </c>
       <c r="D16" s="17" t="s">
-        <v>372</v>
+        <v>368</v>
       </c>
       <c r="E16" s="17" t="s">
         <v>136</v>
@@ -2770,7 +2801,7 @@
         <v>2</v>
       </c>
       <c r="Q16" s="23">
-        <f>SUM(M16:P16)/4</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -2785,7 +2816,7 @@
         <v>184</v>
       </c>
       <c r="D17" s="17" t="s">
-        <v>373</v>
+        <v>369</v>
       </c>
       <c r="E17" s="17" t="s">
         <v>185</v>
@@ -2816,7 +2847,7 @@
         <v>3</v>
       </c>
       <c r="Q17" s="23">
-        <f>SUM(M17:P17)/4</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -2831,7 +2862,7 @@
         <v>218</v>
       </c>
       <c r="D18" s="1" t="s">
-        <v>374</v>
+        <v>370</v>
       </c>
       <c r="E18" s="1" t="s">
         <v>219</v>
@@ -2864,7 +2895,7 @@
         <v>3</v>
       </c>
       <c r="Q18" s="23">
-        <f>SUM(M18:P18)/4</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -2879,7 +2910,7 @@
         <v>333</v>
       </c>
       <c r="D19" s="17" t="s">
-        <v>375</v>
+        <v>371</v>
       </c>
       <c r="E19" s="17" t="s">
         <v>334</v>
@@ -2910,7 +2941,7 @@
         <v>3</v>
       </c>
       <c r="Q19" s="23">
-        <f>SUM(M19:P19)/4</f>
+        <f t="shared" si="0"/>
         <v>2.75</v>
       </c>
     </row>
@@ -2925,7 +2956,7 @@
         <v>39</v>
       </c>
       <c r="D20" s="18" t="s">
-        <v>376</v>
+        <v>372</v>
       </c>
       <c r="E20" s="18" t="s">
         <v>40</v>
@@ -2958,7 +2989,7 @@
         <v>2</v>
       </c>
       <c r="Q20" s="23">
-        <f>SUM(M20:P20)/4</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -2973,7 +3004,7 @@
         <v>43</v>
       </c>
       <c r="D21" s="18" t="s">
-        <v>377</v>
+        <v>373</v>
       </c>
       <c r="E21" s="18" t="s">
         <v>44</v>
@@ -3004,7 +3035,7 @@
         <v>2</v>
       </c>
       <c r="Q21" s="23">
-        <f>SUM(M21:P21)/4</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3019,10 +3050,10 @@
         <v>93</v>
       </c>
       <c r="D22" s="17" t="s">
-        <v>439</v>
+        <v>435</v>
       </c>
       <c r="E22" s="17" t="s">
-        <v>440</v>
+        <v>436</v>
       </c>
       <c r="F22" s="17"/>
       <c r="G22" s="17"/>
@@ -3048,7 +3079,7 @@
         <v>3</v>
       </c>
       <c r="Q22" s="23">
-        <f>SUM(M22:P22)/4</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3063,7 +3094,7 @@
         <v>116</v>
       </c>
       <c r="D23" s="18" t="s">
-        <v>378</v>
+        <v>374</v>
       </c>
       <c r="E23" s="18" t="s">
         <v>117</v>
@@ -3094,7 +3125,7 @@
         <v>3</v>
       </c>
       <c r="Q23" s="23">
-        <f>SUM(M23:P23)/4</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3109,10 +3140,10 @@
         <v>121</v>
       </c>
       <c r="D24" s="17" t="s">
-        <v>441</v>
+        <v>437</v>
       </c>
       <c r="E24" s="17" t="s">
-        <v>442</v>
+        <v>438</v>
       </c>
       <c r="F24" s="17" t="s">
         <v>26</v>
@@ -3142,7 +3173,7 @@
         <v>3</v>
       </c>
       <c r="Q24" s="23">
-        <f>SUM(M24:P24)/4</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3157,7 +3188,7 @@
         <v>160</v>
       </c>
       <c r="D25" s="17" t="s">
-        <v>438</v>
+        <v>434</v>
       </c>
       <c r="E25" s="17" t="s">
         <v>161</v>
@@ -3188,7 +3219,7 @@
         <v>3</v>
       </c>
       <c r="Q25" s="23">
-        <f>SUM(M25:P25)/4</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
@@ -3203,7 +3234,7 @@
         <v>47</v>
       </c>
       <c r="D26" s="18" t="s">
-        <v>379</v>
+        <v>375</v>
       </c>
       <c r="E26" s="18" t="s">
         <v>48</v>
@@ -3234,7 +3265,7 @@
         <v>3</v>
       </c>
       <c r="Q26" s="23">
-        <f>SUM(M26:P26)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3249,7 +3280,7 @@
         <v>81</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>380</v>
+        <v>376</v>
       </c>
       <c r="E27" s="17" t="s">
         <v>82</v>
@@ -3282,7 +3313,7 @@
         <v>3</v>
       </c>
       <c r="Q27" s="23">
-        <f>SUM(M27:P27)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3297,7 +3328,7 @@
         <v>85</v>
       </c>
       <c r="D28" s="17" t="s">
-        <v>381</v>
+        <v>377</v>
       </c>
       <c r="E28" s="17" t="s">
         <v>86</v>
@@ -3328,7 +3359,7 @@
         <v>2</v>
       </c>
       <c r="Q28" s="23">
-        <f>SUM(M28:P28)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3343,7 +3374,7 @@
         <v>104</v>
       </c>
       <c r="D29" s="17" t="s">
-        <v>382</v>
+        <v>378</v>
       </c>
       <c r="E29" s="17" t="s">
         <v>323</v>
@@ -3376,7 +3407,7 @@
         <v>2</v>
       </c>
       <c r="Q29" s="23">
-        <f>SUM(M29:P29)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3391,7 +3422,7 @@
         <v>131</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>383</v>
+        <v>379</v>
       </c>
       <c r="E30" s="18" t="s">
         <v>132</v>
@@ -3422,7 +3453,7 @@
         <v>3</v>
       </c>
       <c r="Q30" s="23">
-        <f>SUM(M30:P30)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3437,7 +3468,7 @@
         <v>143</v>
       </c>
       <c r="D31" s="18" t="s">
-        <v>384</v>
+        <v>380</v>
       </c>
       <c r="E31" s="18" t="s">
         <v>144</v>
@@ -3468,7 +3499,7 @@
         <v>2</v>
       </c>
       <c r="Q31" s="23">
-        <f>SUM(M31:P31)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3483,7 +3514,7 @@
         <v>156</v>
       </c>
       <c r="D32" s="17" t="s">
-        <v>385</v>
+        <v>381</v>
       </c>
       <c r="E32" s="17" t="s">
         <v>157</v>
@@ -3516,7 +3547,7 @@
         <v>2</v>
       </c>
       <c r="Q32" s="23">
-        <f>SUM(M32:P32)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3531,7 +3562,7 @@
         <v>180</v>
       </c>
       <c r="D33" s="17" t="s">
-        <v>386</v>
+        <v>382</v>
       </c>
       <c r="E33" s="17" t="s">
         <v>181</v>
@@ -3560,7 +3591,7 @@
         <v>3</v>
       </c>
       <c r="Q33" s="23">
-        <f>SUM(M33:P33)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3575,7 +3606,7 @@
         <v>238</v>
       </c>
       <c r="D34" s="1" t="s">
-        <v>387</v>
+        <v>383</v>
       </c>
       <c r="E34" s="1" t="s">
         <v>239</v>
@@ -3606,7 +3637,7 @@
         <v>2</v>
       </c>
       <c r="Q34" s="23">
-        <f>SUM(M34:P34)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3621,7 +3652,7 @@
         <v>249</v>
       </c>
       <c r="D35" s="1" t="s">
-        <v>388</v>
+        <v>384</v>
       </c>
       <c r="E35" s="1" t="s">
         <v>250</v>
@@ -3652,7 +3683,7 @@
         <v>3</v>
       </c>
       <c r="Q35" s="23">
-        <f>SUM(M35:P35)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3667,7 +3698,7 @@
         <v>344</v>
       </c>
       <c r="D36" s="17" t="s">
-        <v>389</v>
+        <v>385</v>
       </c>
       <c r="E36" s="17" t="s">
         <v>342</v>
@@ -3698,7 +3729,7 @@
         <v>2</v>
       </c>
       <c r="Q36" s="23">
-        <f>SUM(M36:P36)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
@@ -3713,7 +3744,7 @@
         <v>35</v>
       </c>
       <c r="D37" s="18" t="s">
-        <v>390</v>
+        <v>386</v>
       </c>
       <c r="E37" s="18" t="s">
         <v>36</v>
@@ -3744,7 +3775,7 @@
         <v>3</v>
       </c>
       <c r="Q37" s="23">
-        <f>SUM(M37:P37)/4</f>
+        <f t="shared" ref="Q37:Q68" si="1">SUM(M37:P37)/4</f>
         <v>2</v>
       </c>
     </row>
@@ -3759,7 +3790,7 @@
         <v>68</v>
       </c>
       <c r="D38" s="18" t="s">
-        <v>391</v>
+        <v>387</v>
       </c>
       <c r="E38" s="18" t="s">
         <v>69</v>
@@ -3790,7 +3821,7 @@
         <v>3</v>
       </c>
       <c r="Q38" s="23">
-        <f>SUM(M38:P38)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -3805,7 +3836,7 @@
         <v>77</v>
       </c>
       <c r="D39" s="17" t="s">
-        <v>392</v>
+        <v>388</v>
       </c>
       <c r="E39" s="17" t="s">
         <v>78</v>
@@ -3836,7 +3867,7 @@
         <v>2</v>
       </c>
       <c r="Q39" s="23">
-        <f>SUM(M39:P39)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -3851,7 +3882,7 @@
         <v>100</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>393</v>
+        <v>389</v>
       </c>
       <c r="E40" s="17" t="s">
         <v>101</v>
@@ -3882,7 +3913,7 @@
         <v>2</v>
       </c>
       <c r="Q40" s="23">
-        <f>SUM(M40:P40)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -3897,7 +3928,7 @@
         <v>111</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>394</v>
+        <v>390</v>
       </c>
       <c r="E41" s="18" t="s">
         <v>112</v>
@@ -3928,7 +3959,7 @@
         <v>1</v>
       </c>
       <c r="Q41" s="23">
-        <f>SUM(M41:P41)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -3943,7 +3974,7 @@
         <v>168</v>
       </c>
       <c r="D42" s="18" t="s">
-        <v>395</v>
+        <v>391</v>
       </c>
       <c r="E42" s="18" t="s">
         <v>169</v>
@@ -3976,7 +4007,7 @@
         <v>2</v>
       </c>
       <c r="Q42" s="23">
-        <f>SUM(M42:P42)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -3991,7 +4022,7 @@
         <v>172</v>
       </c>
       <c r="D43" s="17" t="s">
-        <v>396</v>
+        <v>392</v>
       </c>
       <c r="E43" s="17" t="s">
         <v>173</v>
@@ -4022,7 +4053,7 @@
         <v>2</v>
       </c>
       <c r="Q43" s="23">
-        <f>SUM(M43:P43)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4037,7 +4068,7 @@
         <v>214</v>
       </c>
       <c r="D44" s="1" t="s">
-        <v>397</v>
+        <v>393</v>
       </c>
       <c r="E44" s="1" t="s">
         <v>215</v>
@@ -4068,7 +4099,7 @@
         <v>2</v>
       </c>
       <c r="Q44" s="23">
-        <f>SUM(M44:P44)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4083,7 +4114,7 @@
         <v>230</v>
       </c>
       <c r="D45" s="1" t="s">
-        <v>398</v>
+        <v>394</v>
       </c>
       <c r="E45" s="1" t="s">
         <v>231</v>
@@ -4114,7 +4145,7 @@
         <v>2</v>
       </c>
       <c r="Q45" s="23">
-        <f>SUM(M45:P45)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4129,7 +4160,7 @@
         <v>234</v>
       </c>
       <c r="D46" s="1" t="s">
-        <v>399</v>
+        <v>395</v>
       </c>
       <c r="E46" s="1" t="s">
         <v>235</v>
@@ -4160,7 +4191,7 @@
         <v>2</v>
       </c>
       <c r="Q46" s="23">
-        <f>SUM(M46:P46)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4175,7 +4206,7 @@
         <v>303</v>
       </c>
       <c r="D47" s="17" t="s">
-        <v>400</v>
+        <v>396</v>
       </c>
       <c r="E47" s="17" t="s">
         <v>300</v>
@@ -4206,7 +4237,7 @@
         <v>2</v>
       </c>
       <c r="Q47" s="23">
-        <f>SUM(M47:P47)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4221,7 +4252,7 @@
         <v>320</v>
       </c>
       <c r="D48" s="17" t="s">
-        <v>401</v>
+        <v>397</v>
       </c>
       <c r="E48" s="17" t="s">
         <v>321</v>
@@ -4252,7 +4283,7 @@
         <v>2</v>
       </c>
       <c r="Q48" s="23">
-        <f>SUM(M48:P48)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4267,7 +4298,7 @@
         <v>338</v>
       </c>
       <c r="D49" s="17" t="s">
-        <v>402</v>
+        <v>398</v>
       </c>
       <c r="E49" s="17" t="s">
         <v>339</v>
@@ -4298,7 +4329,7 @@
         <v>2</v>
       </c>
       <c r="Q49" s="23">
-        <f>SUM(M49:P49)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4313,7 +4344,7 @@
         <v>347</v>
       </c>
       <c r="D50" s="17" t="s">
-        <v>403</v>
+        <v>399</v>
       </c>
       <c r="E50" s="17" t="s">
         <v>348</v>
@@ -4344,7 +4375,7 @@
         <v>3</v>
       </c>
       <c r="Q50" s="23">
-        <f>SUM(M50:P50)/4</f>
+        <f t="shared" si="1"/>
         <v>2</v>
       </c>
     </row>
@@ -4359,7 +4390,7 @@
         <v>29</v>
       </c>
       <c r="D51" s="18" t="s">
-        <v>404</v>
+        <v>400</v>
       </c>
       <c r="E51" s="18" t="s">
         <v>30</v>
@@ -4392,7 +4423,7 @@
         <v>3</v>
       </c>
       <c r="Q51" s="23">
-        <f>SUM(M51:P51)/4</f>
+        <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
     </row>
@@ -4407,7 +4438,7 @@
         <v>52</v>
       </c>
       <c r="D52" s="18" t="s">
-        <v>405</v>
+        <v>401</v>
       </c>
       <c r="E52" s="18" t="s">
         <v>53</v>
@@ -4436,7 +4467,7 @@
         <v>2</v>
       </c>
       <c r="Q52" s="23">
-        <f>SUM(M52:P52)/4</f>
+        <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
     </row>
@@ -4451,7 +4482,7 @@
         <v>205</v>
       </c>
       <c r="D53" s="17" t="s">
-        <v>406</v>
+        <v>402</v>
       </c>
       <c r="E53" s="17" t="s">
         <v>206</v>
@@ -4484,7 +4515,7 @@
         <v>2</v>
       </c>
       <c r="Q53" s="23">
-        <f>SUM(M53:P53)/4</f>
+        <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
     </row>
@@ -4499,7 +4530,7 @@
         <v>242</v>
       </c>
       <c r="D54" s="1" t="s">
-        <v>407</v>
+        <v>403</v>
       </c>
       <c r="E54" s="1" t="s">
         <v>243</v>
@@ -4528,7 +4559,7 @@
         <v>2</v>
       </c>
       <c r="Q54" s="23">
-        <f>SUM(M54:P54)/4</f>
+        <f t="shared" si="1"/>
         <v>1.75</v>
       </c>
     </row>
@@ -4543,7 +4574,7 @@
         <v>24</v>
       </c>
       <c r="D55" s="17" t="s">
-        <v>408</v>
+        <v>404</v>
       </c>
       <c r="E55" s="17" t="s">
         <v>25</v>
@@ -4574,7 +4605,7 @@
         <v>2</v>
       </c>
       <c r="Q55" s="23">
-        <f>SUM(M55:P55)/4</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -4589,7 +4620,7 @@
         <v>107</v>
       </c>
       <c r="D56" s="17" t="s">
-        <v>409</v>
+        <v>405</v>
       </c>
       <c r="E56" s="17" t="s">
         <v>108</v>
@@ -4620,7 +4651,7 @@
         <v>2</v>
       </c>
       <c r="Q56" s="23">
-        <f>SUM(M56:P56)/4</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -4635,7 +4666,7 @@
         <v>152</v>
       </c>
       <c r="D57" s="17" t="s">
-        <v>410</v>
+        <v>406</v>
       </c>
       <c r="E57" s="17" t="s">
         <v>153</v>
@@ -4668,7 +4699,7 @@
         <v>2</v>
       </c>
       <c r="Q57" s="23">
-        <f>SUM(M57:P57)/4</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -4683,7 +4714,7 @@
         <v>201</v>
       </c>
       <c r="D58" s="17" t="s">
-        <v>411</v>
+        <v>407</v>
       </c>
       <c r="E58" s="17" t="s">
         <v>202</v>
@@ -4714,7 +4745,7 @@
         <v>2</v>
       </c>
       <c r="Q58" s="23">
-        <f>SUM(M58:P58)/4</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -4729,7 +4760,7 @@
         <v>226</v>
       </c>
       <c r="D59" s="1" t="s">
-        <v>412</v>
+        <v>408</v>
       </c>
       <c r="E59" s="1" t="s">
         <v>227</v>
@@ -4761,7 +4792,7 @@
         <v>2</v>
       </c>
       <c r="Q59" s="23">
-        <f>SUM(M59:P59)/4</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -4776,7 +4807,7 @@
         <v>304</v>
       </c>
       <c r="D60" s="17" t="s">
-        <v>413</v>
+        <v>409</v>
       </c>
       <c r="E60" s="17" t="s">
         <v>308</v>
@@ -4807,7 +4838,7 @@
         <v>1</v>
       </c>
       <c r="Q60" s="23">
-        <f>SUM(M60:P60)/4</f>
+        <f t="shared" si="1"/>
         <v>1.5</v>
       </c>
     </row>
@@ -4822,7 +4853,7 @@
         <v>73</v>
       </c>
       <c r="D61" s="17" t="s">
-        <v>414</v>
+        <v>410</v>
       </c>
       <c r="E61" s="17" t="s">
         <v>74</v>
@@ -4853,7 +4884,7 @@
         <v>1</v>
       </c>
       <c r="Q61" s="23">
-        <f>SUM(M61:P61)/4</f>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
@@ -4868,7 +4899,7 @@
         <v>164</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>415</v>
+        <v>411</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>165</v>
@@ -4901,7 +4932,7 @@
         <v>1</v>
       </c>
       <c r="Q62" s="23">
-        <f>SUM(M62:P62)/4</f>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
@@ -4916,7 +4947,7 @@
         <v>189</v>
       </c>
       <c r="D63" s="17" t="s">
-        <v>416</v>
+        <v>412</v>
       </c>
       <c r="E63" s="17" t="s">
         <v>190</v>
@@ -4947,7 +4978,7 @@
         <v>2</v>
       </c>
       <c r="Q63" s="23">
-        <f>SUM(M63:P63)/4</f>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
@@ -4962,7 +4993,7 @@
         <v>222</v>
       </c>
       <c r="D64" s="1" t="s">
-        <v>417</v>
+        <v>413</v>
       </c>
       <c r="E64" s="1" t="s">
         <v>223</v>
@@ -4995,7 +5026,7 @@
         <v>1</v>
       </c>
       <c r="Q64" s="23">
-        <f>SUM(M64:P64)/4</f>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
@@ -5010,7 +5041,7 @@
         <v>307</v>
       </c>
       <c r="D65" s="17" t="s">
-        <v>418</v>
+        <v>414</v>
       </c>
       <c r="E65" s="17" t="s">
         <v>309</v>
@@ -5041,7 +5072,7 @@
         <v>1</v>
       </c>
       <c r="Q65" s="23">
-        <f>SUM(M65:P65)/4</f>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
@@ -5056,7 +5087,7 @@
         <v>313</v>
       </c>
       <c r="D66" s="36" t="s">
-        <v>419</v>
+        <v>415</v>
       </c>
       <c r="E66" s="17" t="s">
         <v>328</v>
@@ -5087,7 +5118,7 @@
         <v>2</v>
       </c>
       <c r="Q66" s="23">
-        <f>SUM(M66:P66)/4</f>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
@@ -5102,7 +5133,7 @@
         <v>325</v>
       </c>
       <c r="D67" s="17" t="s">
-        <v>420</v>
+        <v>416</v>
       </c>
       <c r="E67" s="17" t="s">
         <v>326</v>
@@ -5133,7 +5164,7 @@
         <v>2</v>
       </c>
       <c r="Q67" s="23">
-        <f>SUM(M67:P67)/4</f>
+        <f t="shared" si="1"/>
         <v>1.25</v>
       </c>
     </row>
@@ -5148,7 +5179,7 @@
         <v>18</v>
       </c>
       <c r="D68" s="17" t="s">
-        <v>421</v>
+        <v>417</v>
       </c>
       <c r="E68" s="17" t="s">
         <v>19</v>
@@ -5179,7 +5210,7 @@
         <v>1</v>
       </c>
       <c r="Q68" s="23">
-        <f>SUM(M68:P68)/4</f>
+        <f t="shared" si="1"/>
         <v>1</v>
       </c>
     </row>
@@ -5194,7 +5225,7 @@
         <v>176</v>
       </c>
       <c r="D69" s="17" t="s">
-        <v>422</v>
+        <v>418</v>
       </c>
       <c r="E69" s="17" t="s">
         <v>177</v>
@@ -5225,7 +5256,7 @@
         <v>1</v>
       </c>
       <c r="Q69" s="23">
-        <f>SUM(M69:P69)/4</f>
+        <f t="shared" ref="Q69:Q100" si="2">SUM(M69:P69)/4</f>
         <v>1</v>
       </c>
     </row>
@@ -5240,7 +5271,7 @@
         <v>193</v>
       </c>
       <c r="D70" s="17" t="s">
-        <v>423</v>
+        <v>419</v>
       </c>
       <c r="E70" s="17" t="s">
         <v>194</v>
@@ -5271,7 +5302,7 @@
         <v>1</v>
       </c>
       <c r="Q70" s="23">
-        <f>SUM(M70:P70)/4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5286,7 +5317,7 @@
         <v>197</v>
       </c>
       <c r="D71" s="17" t="s">
-        <v>424</v>
+        <v>420</v>
       </c>
       <c r="E71" s="17" t="s">
         <v>198</v>
@@ -5317,7 +5348,7 @@
         <v>1</v>
       </c>
       <c r="Q71" s="23">
-        <f>SUM(M71:P71)/4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5332,7 +5363,7 @@
         <v>246</v>
       </c>
       <c r="D72" s="1" t="s">
-        <v>425</v>
+        <v>421</v>
       </c>
       <c r="E72" s="1" t="s">
         <v>247</v>
@@ -5363,7 +5394,7 @@
         <v>1</v>
       </c>
       <c r="Q72" s="23">
-        <f>SUM(M72:P72)/4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5378,7 +5409,7 @@
         <v>296</v>
       </c>
       <c r="D73" s="17" t="s">
-        <v>426</v>
+        <v>422</v>
       </c>
       <c r="E73" s="17" t="s">
         <v>297</v>
@@ -5409,7 +5440,7 @@
         <v>1</v>
       </c>
       <c r="Q73" s="23">
-        <f>SUM(M73:P73)/4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5424,7 +5455,7 @@
         <v>317</v>
       </c>
       <c r="D74" s="17" t="s">
-        <v>427</v>
+        <v>423</v>
       </c>
       <c r="E74" s="17" t="s">
         <v>345</v>
@@ -5455,7 +5486,7 @@
         <v>1</v>
       </c>
       <c r="Q74" s="23">
-        <f>SUM(M74:P74)/4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5470,7 +5501,7 @@
         <v>330</v>
       </c>
       <c r="D75" s="17" t="s">
-        <v>428</v>
+        <v>424</v>
       </c>
       <c r="E75" s="17" t="s">
         <v>331</v>
@@ -5501,7 +5532,7 @@
         <v>1</v>
       </c>
       <c r="Q75" s="23">
-        <f>SUM(M75:P75)/4</f>
+        <f t="shared" si="2"/>
         <v>1</v>
       </c>
     </row>
@@ -5623,10 +5654,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
-  <dimension ref="A1:O114"/>
+  <dimension ref="A1:P113"/>
   <sheetViews>
-    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -5646,7 +5677,7 @@
     <col min="15" max="15" width="5.7109375" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A1" s="30" t="s">
         <v>0</v>
       </c>
@@ -5664,7 +5695,7 @@
       <c r="N1" s="35"/>
       <c r="O1" s="35"/>
     </row>
-    <row r="2" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A2" s="31" t="s">
         <v>252</v>
       </c>
@@ -5683,7 +5714,7 @@
       <c r="N2" s="35"/>
       <c r="O2" s="35"/>
     </row>
-    <row r="3" spans="1:15" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:16" x14ac:dyDescent="0.2">
       <c r="A3" s="36"/>
       <c r="B3" s="36"/>
       <c r="C3" s="36"/>
@@ -5704,7 +5735,7 @@
       <c r="N3" s="35"/>
       <c r="O3" s="8"/>
     </row>
-    <row r="4" spans="1:15" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:16" ht="28.15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>4</v>
       </c>
@@ -5751,7 +5782,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="5" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="34">
         <v>1</v>
       </c>
@@ -5762,7 +5793,7 @@
         <v>255</v>
       </c>
       <c r="D5" s="18" t="s">
-        <v>256</v>
+        <v>439</v>
       </c>
       <c r="E5" s="18" t="s">
         <v>256</v>
@@ -5789,198 +5820,201 @@
         <v>3</v>
       </c>
       <c r="O5" s="23">
-        <f>SUM(K5:N5)/4</f>
+        <f t="shared" ref="O5:O18" si="0">SUM(K5:N5)/4</f>
         <v>3.25</v>
       </c>
-    </row>
-    <row r="6" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="P5" s="44"/>
+    </row>
+    <row r="6" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="34">
         <v>2</v>
       </c>
-      <c r="B6" s="18" t="s">
-        <v>254</v>
-      </c>
-      <c r="C6" s="18" t="s">
-        <v>255</v>
-      </c>
-      <c r="D6" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="E6" s="18" t="s">
-        <v>367</v>
-      </c>
-      <c r="F6" s="17" t="s">
-        <v>257</v>
+      <c r="B6" s="39" t="s">
+        <v>267</v>
+      </c>
+      <c r="C6" s="39" t="s">
+        <v>268</v>
+      </c>
+      <c r="D6" s="40" t="s">
+        <v>440</v>
+      </c>
+      <c r="E6" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="F6" s="39" t="s">
+        <v>270</v>
       </c>
       <c r="G6" s="19"/>
-      <c r="H6" s="20"/>
-      <c r="I6" s="20"/>
+      <c r="H6" s="38"/>
+      <c r="I6" s="38"/>
       <c r="J6" s="21" t="s">
         <v>22</v>
       </c>
       <c r="K6" s="22">
-        <v>4</v>
-      </c>
-      <c r="L6" s="16">
-        <v>3</v>
-      </c>
-      <c r="M6" s="16">
-        <v>3</v>
+        <v>3</v>
+      </c>
+      <c r="L6" s="22">
+        <v>3</v>
+      </c>
+      <c r="M6" s="22">
+        <v>2</v>
       </c>
       <c r="N6" s="22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O6" s="23">
-        <f>SUM(K6:N6)/4</f>
-        <v>3.25</v>
-      </c>
-    </row>
-    <row r="7" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="34">
         <v>3</v>
       </c>
-      <c r="B7" s="39" t="s">
-        <v>267</v>
-      </c>
-      <c r="C7" s="39" t="s">
-        <v>268</v>
-      </c>
-      <c r="D7" s="40" t="s">
-        <v>269</v>
-      </c>
-      <c r="E7" s="40" t="s">
-        <v>269</v>
-      </c>
-      <c r="F7" s="39" t="s">
-        <v>270</v>
-      </c>
-      <c r="G7" s="19"/>
-      <c r="H7" s="38"/>
-      <c r="I7" s="38"/>
-      <c r="J7" s="21" t="s">
-        <v>22</v>
-      </c>
+      <c r="B7" s="17" t="s">
+        <v>271</v>
+      </c>
+      <c r="C7" s="18" t="s">
+        <v>272</v>
+      </c>
+      <c r="D7" s="17" t="s">
+        <v>441</v>
+      </c>
+      <c r="E7" s="18" t="s">
+        <v>273</v>
+      </c>
+      <c r="F7" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="G7" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H7" s="20"/>
+      <c r="I7" s="20"/>
+      <c r="J7" s="21"/>
       <c r="K7" s="22">
         <v>3</v>
       </c>
-      <c r="L7" s="22">
-        <v>3</v>
-      </c>
-      <c r="M7" s="22">
-        <v>2</v>
+      <c r="L7" s="16">
+        <v>2</v>
+      </c>
+      <c r="M7" s="16">
+        <v>3</v>
       </c>
       <c r="N7" s="22">
         <v>2</v>
       </c>
       <c r="O7" s="23">
-        <f>SUM(K7:N7)/4</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="8" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="34">
         <v>4</v>
       </c>
       <c r="B8" s="17" t="s">
-        <v>271</v>
-      </c>
-      <c r="C8" s="18" t="s">
-        <v>272</v>
-      </c>
-      <c r="D8" s="17" t="s">
-        <v>368</v>
+        <v>291</v>
+      </c>
+      <c r="C8" s="17" t="s">
+        <v>292</v>
+      </c>
+      <c r="D8" s="18" t="s">
+        <v>442</v>
       </c>
       <c r="E8" s="18" t="s">
-        <v>273</v>
+        <v>293</v>
       </c>
       <c r="F8" s="17" t="s">
-        <v>274</v>
-      </c>
-      <c r="G8" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="H8" s="20"/>
+        <v>294</v>
+      </c>
+      <c r="G8" s="19"/>
+      <c r="H8" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="I8" s="20"/>
       <c r="J8" s="21"/>
-      <c r="K8" s="22">
-        <v>3</v>
-      </c>
-      <c r="L8" s="16">
-        <v>2</v>
-      </c>
-      <c r="M8" s="16">
-        <v>3</v>
-      </c>
-      <c r="N8" s="22">
-        <v>2</v>
+      <c r="K8" s="35">
+        <v>2</v>
+      </c>
+      <c r="L8" s="36">
+        <v>2</v>
+      </c>
+      <c r="M8" s="36">
+        <v>3</v>
+      </c>
+      <c r="N8" s="35">
+        <v>3</v>
       </c>
       <c r="O8" s="23">
-        <f>SUM(K8:N8)/4</f>
+        <f t="shared" si="0"/>
         <v>2.5</v>
       </c>
     </row>
-    <row r="9" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="34">
         <v>5</v>
       </c>
       <c r="B9" s="17" t="s">
-        <v>291</v>
+        <v>259</v>
       </c>
       <c r="C9" s="17" t="s">
-        <v>292</v>
+        <v>258</v>
       </c>
       <c r="D9" s="18" t="s">
-        <v>293</v>
+        <v>443</v>
       </c>
       <c r="E9" s="18" t="s">
-        <v>293</v>
+        <v>260</v>
       </c>
       <c r="F9" s="17" t="s">
-        <v>294</v>
+        <v>261</v>
       </c>
       <c r="G9" s="19"/>
-      <c r="H9" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="H9" s="20"/>
       <c r="I9" s="20"/>
-      <c r="J9" s="21"/>
-      <c r="K9" s="35">
-        <v>2</v>
-      </c>
-      <c r="L9" s="36">
-        <v>2</v>
-      </c>
-      <c r="M9" s="36">
-        <v>3</v>
-      </c>
-      <c r="N9" s="35">
-        <v>3</v>
+      <c r="J9" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K9" s="22">
+        <v>3</v>
+      </c>
+      <c r="L9" s="16">
+        <v>2</v>
+      </c>
+      <c r="M9" s="16">
+        <v>2</v>
+      </c>
+      <c r="N9" s="22">
+        <v>2</v>
       </c>
       <c r="O9" s="23">
-        <f>SUM(K9:N9)/4</f>
-        <v>2.5</v>
-      </c>
-    </row>
-    <row r="10" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="34">
         <v>6</v>
       </c>
       <c r="B10" s="17" t="s">
-        <v>259</v>
-      </c>
-      <c r="C10" s="17" t="s">
-        <v>258</v>
-      </c>
-      <c r="D10" s="18" t="s">
-        <v>260</v>
+        <v>262</v>
+      </c>
+      <c r="C10" s="18" t="s">
+        <v>263</v>
+      </c>
+      <c r="D10" s="17" t="s">
+        <v>444</v>
       </c>
       <c r="E10" s="18" t="s">
-        <v>260</v>
+        <v>264</v>
       </c>
       <c r="F10" s="17" t="s">
-        <v>261</v>
-      </c>
-      <c r="G10" s="19"/>
+        <v>265</v>
+      </c>
+      <c r="G10" s="25" t="s">
+        <v>22</v>
+      </c>
       <c r="H10" s="20"/>
       <c r="I10" s="20"/>
       <c r="J10" s="21" t="s">
@@ -5990,134 +6024,132 @@
         <v>3</v>
       </c>
       <c r="L10" s="16">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="M10" s="16">
         <v>2</v>
       </c>
       <c r="N10" s="22">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="O10" s="23">
-        <f>SUM(K10:N10)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
-    <row r="11" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="34">
         <v>7</v>
       </c>
       <c r="B11" s="17" t="s">
-        <v>262</v>
-      </c>
-      <c r="C11" s="18" t="s">
-        <v>263</v>
-      </c>
-      <c r="D11" s="17" t="s">
-        <v>369</v>
+        <v>283</v>
+      </c>
+      <c r="C11" s="17" t="s">
+        <v>284</v>
+      </c>
+      <c r="D11" s="18" t="s">
+        <v>445</v>
       </c>
       <c r="E11" s="18" t="s">
-        <v>264</v>
+        <v>285</v>
       </c>
       <c r="F11" s="17" t="s">
-        <v>265</v>
-      </c>
-      <c r="G11" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="H11" s="20"/>
+        <v>286</v>
+      </c>
+      <c r="G11" s="19"/>
+      <c r="H11" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="I11" s="20"/>
-      <c r="J11" s="21" t="s">
-        <v>22</v>
-      </c>
-      <c r="K11" s="22">
-        <v>3</v>
-      </c>
-      <c r="L11" s="16">
-        <v>3</v>
-      </c>
-      <c r="M11" s="16">
-        <v>2</v>
-      </c>
-      <c r="N11" s="22">
-        <v>1</v>
+      <c r="J11" s="21"/>
+      <c r="K11" s="35">
+        <v>2</v>
+      </c>
+      <c r="L11" s="36">
+        <v>3</v>
+      </c>
+      <c r="M11" s="36">
+        <v>2</v>
+      </c>
+      <c r="N11" s="35">
+        <v>2</v>
       </c>
       <c r="O11" s="23">
-        <f>SUM(K11:N11)/4</f>
+        <f t="shared" si="0"/>
         <v>2.25</v>
       </c>
     </row>
-    <row r="12" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:16" ht="60" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="34">
         <v>8</v>
       </c>
       <c r="B12" s="17" t="s">
-        <v>283</v>
+        <v>266</v>
       </c>
       <c r="C12" s="17" t="s">
-        <v>284</v>
-      </c>
-      <c r="D12" s="18" t="s">
-        <v>285</v>
+        <v>364</v>
+      </c>
+      <c r="D12" s="17" t="s">
+        <v>446</v>
       </c>
       <c r="E12" s="18" t="s">
-        <v>285</v>
-      </c>
-      <c r="F12" s="17" t="s">
-        <v>286</v>
-      </c>
-      <c r="G12" s="19"/>
-      <c r="H12" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I12" s="20"/>
-      <c r="J12" s="21"/>
-      <c r="K12" s="35">
-        <v>2</v>
-      </c>
-      <c r="L12" s="36">
-        <v>3</v>
-      </c>
-      <c r="M12" s="36">
-        <v>2</v>
-      </c>
-      <c r="N12" s="35">
+        <v>365</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>83</v>
+      </c>
+      <c r="G12" s="25" t="s">
+        <v>22</v>
+      </c>
+      <c r="H12" s="20"/>
+      <c r="I12" s="20" t="s">
+        <v>22</v>
+      </c>
+      <c r="J12" s="21" t="s">
+        <v>22</v>
+      </c>
+      <c r="K12" s="22">
+        <v>2</v>
+      </c>
+      <c r="L12" s="16">
+        <v>2</v>
+      </c>
+      <c r="M12" s="16">
+        <v>1</v>
+      </c>
+      <c r="N12" s="22">
         <v>2</v>
       </c>
       <c r="O12" s="23">
-        <f>SUM(K12:N12)/4</f>
-        <v>2.25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:15" ht="60" customHeight="1" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" ht="38.25" x14ac:dyDescent="0.2">
       <c r="A13" s="34">
         <v>9</v>
       </c>
       <c r="B13" s="17" t="s">
-        <v>266</v>
+        <v>275</v>
       </c>
       <c r="C13" s="17" t="s">
-        <v>365</v>
-      </c>
-      <c r="D13" s="17" t="s">
-        <v>364</v>
+        <v>276</v>
+      </c>
+      <c r="D13" s="18" t="s">
+        <v>447</v>
       </c>
       <c r="E13" s="18" t="s">
-        <v>366</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>83</v>
+        <v>277</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>278</v>
       </c>
       <c r="G13" s="25" t="s">
         <v>22</v>
       </c>
       <c r="H13" s="20"/>
-      <c r="I13" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="J13" s="21" t="s">
-        <v>22</v>
-      </c>
+      <c r="I13" s="20"/>
+      <c r="J13" s="21"/>
       <c r="K13" s="22">
         <v>2</v>
       </c>
@@ -6131,173 +6163,171 @@
         <v>2</v>
       </c>
       <c r="O13" s="23">
-        <f>SUM(K13:N13)/4</f>
+        <f t="shared" si="0"/>
         <v>1.75</v>
       </c>
     </row>
-    <row r="14" spans="1:15" ht="38.25" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A14" s="34">
         <v>10</v>
       </c>
       <c r="B14" s="17" t="s">
-        <v>275</v>
+        <v>287</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>276</v>
+        <v>288</v>
       </c>
       <c r="D14" s="18" t="s">
-        <v>277</v>
+        <v>448</v>
       </c>
       <c r="E14" s="18" t="s">
-        <v>277</v>
+        <v>289</v>
       </c>
       <c r="F14" s="17" t="s">
-        <v>278</v>
-      </c>
-      <c r="G14" s="25" t="s">
-        <v>22</v>
-      </c>
-      <c r="H14" s="20"/>
+        <v>290</v>
+      </c>
+      <c r="G14" s="19"/>
+      <c r="H14" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="I14" s="20"/>
       <c r="J14" s="21"/>
-      <c r="K14" s="22">
-        <v>2</v>
-      </c>
-      <c r="L14" s="16">
-        <v>2</v>
-      </c>
-      <c r="M14" s="16">
-        <v>1</v>
-      </c>
-      <c r="N14" s="22">
+      <c r="K14" s="35">
+        <v>1</v>
+      </c>
+      <c r="L14" s="36">
+        <v>2</v>
+      </c>
+      <c r="M14" s="36">
+        <v>1</v>
+      </c>
+      <c r="N14" s="35">
         <v>2</v>
       </c>
       <c r="O14" s="23">
-        <f>SUM(K14:N14)/4</f>
-        <v>1.75</v>
-      </c>
-    </row>
-    <row r="15" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" ht="51" x14ac:dyDescent="0.2">
       <c r="A15" s="34">
         <v>11</v>
       </c>
       <c r="B15" s="17" t="s">
-        <v>287</v>
+        <v>356</v>
       </c>
       <c r="C15" s="17" t="s">
-        <v>288</v>
+        <v>357</v>
       </c>
       <c r="D15" s="18" t="s">
-        <v>289</v>
+        <v>449</v>
       </c>
       <c r="E15" s="18" t="s">
-        <v>289</v>
+        <v>358</v>
       </c>
       <c r="F15" s="17" t="s">
-        <v>290</v>
+        <v>363</v>
       </c>
       <c r="G15" s="19"/>
-      <c r="H15" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="I15" s="20"/>
+      <c r="H15" s="20"/>
+      <c r="I15" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="J15" s="21"/>
       <c r="K15" s="35">
-        <v>1</v>
-      </c>
-      <c r="L15" s="36">
-        <v>2</v>
-      </c>
+        <v>2</v>
+      </c>
+      <c r="L15" s="36"/>
       <c r="M15" s="36">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="N15" s="35">
         <v>2</v>
       </c>
       <c r="O15" s="23">
-        <f>SUM(K15:N15)/4</f>
+        <f t="shared" si="0"/>
         <v>1.5</v>
       </c>
     </row>
-    <row r="16" spans="1:15" ht="51" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:16" ht="76.5" x14ac:dyDescent="0.2">
       <c r="A16" s="34">
         <v>12</v>
       </c>
-      <c r="B16" s="17" t="s">
-        <v>356</v>
-      </c>
-      <c r="C16" s="17" t="s">
-        <v>357</v>
+      <c r="B16" s="18" t="s">
+        <v>279</v>
+      </c>
+      <c r="C16" s="18" t="s">
+        <v>280</v>
       </c>
       <c r="D16" s="18" t="s">
-        <v>358</v>
+        <v>450</v>
       </c>
       <c r="E16" s="18" t="s">
-        <v>358</v>
-      </c>
-      <c r="F16" s="17" t="s">
-        <v>363</v>
-      </c>
-      <c r="G16" s="19"/>
+        <v>281</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>282</v>
+      </c>
+      <c r="G16" s="25" t="s">
+        <v>22</v>
+      </c>
       <c r="H16" s="20"/>
-      <c r="I16" s="20" t="s">
-        <v>22</v>
-      </c>
+      <c r="I16" s="20"/>
       <c r="J16" s="21"/>
-      <c r="K16" s="35">
-        <v>2</v>
-      </c>
-      <c r="L16" s="36"/>
-      <c r="M16" s="36">
-        <v>2</v>
-      </c>
-      <c r="N16" s="35">
-        <v>2</v>
+      <c r="K16" s="22">
+        <v>1</v>
+      </c>
+      <c r="L16" s="16">
+        <v>1</v>
+      </c>
+      <c r="M16" s="16">
+        <v>2</v>
+      </c>
+      <c r="N16" s="22">
+        <v>1</v>
       </c>
       <c r="O16" s="23">
-        <f>SUM(K16:N16)/4</f>
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="17" spans="1:15" ht="76.5" x14ac:dyDescent="0.2">
+        <f t="shared" si="0"/>
+        <v>1.25</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
       <c r="A17" s="34">
         <v>13</v>
       </c>
-      <c r="B17" s="18" t="s">
-        <v>279</v>
-      </c>
-      <c r="C17" s="18" t="s">
-        <v>280</v>
+      <c r="B17" s="17" t="s">
+        <v>352</v>
+      </c>
+      <c r="C17" s="17" t="s">
+        <v>353</v>
       </c>
       <c r="D17" s="18" t="s">
-        <v>281</v>
+        <v>451</v>
       </c>
       <c r="E17" s="18" t="s">
-        <v>281</v>
-      </c>
-      <c r="F17" s="18" t="s">
-        <v>282</v>
-      </c>
-      <c r="G17" s="25" t="s">
-        <v>22</v>
-      </c>
+        <v>354</v>
+      </c>
+      <c r="F17" s="17" t="s">
+        <v>355</v>
+      </c>
+      <c r="G17" s="19"/>
       <c r="H17" s="20"/>
-      <c r="I17" s="20"/>
+      <c r="I17" s="20" t="s">
+        <v>22</v>
+      </c>
       <c r="J17" s="21"/>
-      <c r="K17" s="22">
-        <v>1</v>
-      </c>
-      <c r="L17" s="16">
-        <v>1</v>
-      </c>
-      <c r="M17" s="16">
-        <v>2</v>
-      </c>
-      <c r="N17" s="22">
-        <v>1</v>
+      <c r="K17" s="35">
+        <v>1</v>
+      </c>
+      <c r="L17" s="36"/>
+      <c r="M17" s="36">
+        <v>2</v>
+      </c>
+      <c r="N17" s="35">
+        <v>2</v>
       </c>
       <c r="O17" s="23">
-        <f>SUM(K17:N17)/4</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
     </row>
@@ -6306,19 +6336,19 @@
         <v>14</v>
       </c>
       <c r="B18" s="17" t="s">
-        <v>352</v>
+        <v>360</v>
       </c>
       <c r="C18" s="17" t="s">
-        <v>353</v>
+        <v>361</v>
       </c>
       <c r="D18" s="18" t="s">
-        <v>354</v>
+        <v>452</v>
       </c>
       <c r="E18" s="18" t="s">
-        <v>354</v>
+        <v>362</v>
       </c>
       <c r="F18" s="17" t="s">
-        <v>355</v>
+        <v>359</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="20"/>
@@ -6337,66 +6367,30 @@
         <v>2</v>
       </c>
       <c r="O18" s="23">
-        <f>SUM(K18:N18)/4</f>
+        <f t="shared" si="0"/>
         <v>1.25</v>
       </c>
     </row>
-    <row r="19" spans="1:15" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A19" s="34">
-        <v>15</v>
-      </c>
-      <c r="B19" s="17" t="s">
-        <v>360</v>
-      </c>
-      <c r="C19" s="17" t="s">
-        <v>361</v>
-      </c>
-      <c r="D19" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="E19" s="18" t="s">
-        <v>362</v>
-      </c>
-      <c r="F19" s="17" t="s">
-        <v>359</v>
-      </c>
-      <c r="G19" s="19"/>
-      <c r="H19" s="20"/>
-      <c r="I19" s="20" t="s">
-        <v>22</v>
-      </c>
-      <c r="J19" s="21"/>
-      <c r="K19" s="35">
-        <v>1</v>
-      </c>
-      <c r="L19" s="36"/>
-      <c r="M19" s="36">
-        <v>2</v>
-      </c>
-      <c r="N19" s="35">
-        <v>2</v>
-      </c>
-      <c r="O19" s="23">
-        <f>SUM(K19:N19)/4</f>
-        <v>1.25</v>
-      </c>
+    <row r="19" spans="1:15" x14ac:dyDescent="0.2">
+      <c r="A19" s="34"/>
+      <c r="B19" s="17"/>
+      <c r="C19" s="17"/>
+      <c r="D19" s="17"/>
+      <c r="E19" s="18"/>
+      <c r="F19" s="17"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19"/>
+      <c r="K19"/>
+      <c r="L19"/>
+      <c r="M19"/>
+      <c r="N19"/>
+      <c r="O19"/>
     </row>
     <row r="20" spans="1:15" x14ac:dyDescent="0.2">
-      <c r="A20" s="34"/>
       <c r="B20" s="17"/>
       <c r="C20" s="17"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="18"/>
-      <c r="F20" s="17"/>
-      <c r="G20"/>
-      <c r="H20"/>
-      <c r="I20"/>
-      <c r="J20"/>
-      <c r="K20"/>
-      <c r="L20"/>
-      <c r="M20"/>
-      <c r="N20"/>
-      <c r="O20"/>
     </row>
     <row r="21" spans="1:15" x14ac:dyDescent="0.2">
       <c r="B21" s="17"/>
@@ -6531,7 +6525,6 @@
       <c r="C53" s="17"/>
     </row>
     <row r="54" spans="2:3" x14ac:dyDescent="0.2">
-      <c r="B54" s="17"/>
       <c r="C54" s="17"/>
     </row>
     <row r="55" spans="2:3" x14ac:dyDescent="0.2">
@@ -6711,11 +6704,8 @@
     <row r="113" spans="3:3" x14ac:dyDescent="0.2">
       <c r="C113" s="17"/>
     </row>
-    <row r="114" spans="3:3" x14ac:dyDescent="0.2">
-      <c r="C114" s="17"/>
-    </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:O19">
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A5:O18">
     <sortCondition descending="1" ref="O5"/>
   </sortState>
   <phoneticPr fontId="6" type="noConversion"/>

</xml_diff>